<commit_message>
all test scenarios described
</commit_message>
<xml_diff>
--- a/blue-green/aksrgsample/AKS Upgrade.xlsx
+++ b/blue-green/aksrgsample/AKS Upgrade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Chaminda\github\terraform_samples\blue-green\aksrgsample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B65E775-FDF4-4B3A-B345-C4753DE716E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340663CB-EFE2-44B1-8C96-3B84650233DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{783D4FFA-E4BF-4C40-98DC-85ACE5E37AF6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="33">
   <si>
     <t>Phase</t>
   </si>
@@ -83,12 +83,6 @@
     <t>1.25.6</t>
   </si>
   <si>
-    <t>blue deployment</t>
-  </si>
-  <si>
-    <t>green deployment</t>
-  </si>
-  <si>
     <t>1.26.3</t>
   </si>
   <si>
@@ -117,6 +111,30 @@
   </si>
   <si>
     <t>003. blue deployment</t>
+  </si>
+  <si>
+    <t>004. green deployment</t>
+  </si>
+  <si>
+    <t>005. blue deployment - aks upgrade to k8s 1.25.6</t>
+  </si>
+  <si>
+    <t>006. green deployment</t>
+  </si>
+  <si>
+    <t>007. blue deployment</t>
+  </si>
+  <si>
+    <t>008. green deployment - aks upgrade to 1.26.3</t>
+  </si>
+  <si>
+    <t>009. blue deployment - aks upgrade to 1.27.1</t>
+  </si>
+  <si>
+    <t>010. green deployment</t>
+  </si>
+  <si>
+    <t>010. blue deployment</t>
   </si>
 </sst>
 </file>
@@ -498,8 +516,8 @@
   <dimension ref="A1:Q58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,7 +549,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="1"/>
       <c r="M1" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -575,12 +593,12 @@
         <v>10</v>
       </c>
       <c r="Q2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -600,7 +618,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -641,7 +659,7 @@
         <v>6</v>
       </c>
       <c r="Q6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -682,7 +700,7 @@
         <v>4</v>
       </c>
       <c r="Q7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -723,12 +741,12 @@
         <v>4</v>
       </c>
       <c r="Q8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -769,7 +787,7 @@
         <v>4</v>
       </c>
       <c r="Q11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -810,7 +828,7 @@
         <v>4</v>
       </c>
       <c r="Q12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -851,12 +869,12 @@
         <v>4</v>
       </c>
       <c r="Q13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -897,7 +915,7 @@
         <v>4</v>
       </c>
       <c r="Q16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
@@ -938,7 +956,7 @@
         <v>4</v>
       </c>
       <c r="Q17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
@@ -979,12 +997,12 @@
         <v>4</v>
       </c>
       <c r="Q18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
@@ -1025,7 +1043,7 @@
         <v>4</v>
       </c>
       <c r="Q21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
@@ -1066,7 +1084,7 @@
         <v>4</v>
       </c>
       <c r="Q22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
@@ -1107,12 +1125,12 @@
         <v>4</v>
       </c>
       <c r="Q23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
@@ -1153,7 +1171,7 @@
         <v>4</v>
       </c>
       <c r="Q26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
@@ -1194,7 +1212,7 @@
         <v>14</v>
       </c>
       <c r="Q27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
@@ -1235,12 +1253,12 @@
         <v>14</v>
       </c>
       <c r="Q28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
@@ -1281,7 +1299,7 @@
         <v>14</v>
       </c>
       <c r="Q31" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
@@ -1322,7 +1340,7 @@
         <v>14</v>
       </c>
       <c r="Q32" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
@@ -1363,12 +1381,12 @@
         <v>14</v>
       </c>
       <c r="Q33" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
@@ -1409,7 +1427,7 @@
         <v>14</v>
       </c>
       <c r="Q36" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
@@ -1450,7 +1468,7 @@
         <v>14</v>
       </c>
       <c r="Q37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
@@ -1491,12 +1509,12 @@
         <v>14</v>
       </c>
       <c r="Q38" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
@@ -1516,13 +1534,13 @@
         <v>14</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M41">
         <v>1</v>
@@ -1537,7 +1555,7 @@
         <v>14</v>
       </c>
       <c r="Q41" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
@@ -1557,13 +1575,13 @@
         <v>14</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M42">
         <v>0</v>
@@ -1575,10 +1593,10 @@
         <v>1</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q42" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
@@ -1595,16 +1613,16 @@
         <v>1</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M43">
         <v>1</v>
@@ -1616,15 +1634,15 @@
         <v>1</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q43" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
@@ -1641,16 +1659,16 @@
         <v>1</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M46">
         <v>1</v>
@@ -1662,10 +1680,10 @@
         <v>0</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q46" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
@@ -1682,16 +1700,16 @@
         <v>0</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M47">
         <v>1</v>
@@ -1703,10 +1721,10 @@
         <v>0</v>
       </c>
       <c r="P47" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Q47" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
@@ -1723,16 +1741,16 @@
         <v>0</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M48">
         <v>1</v>
@@ -1744,15 +1762,15 @@
         <v>0</v>
       </c>
       <c r="P48" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Q48" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
@@ -1769,16 +1787,16 @@
         <v>0</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M51">
         <v>1</v>
@@ -1790,10 +1808,10 @@
         <v>1</v>
       </c>
       <c r="P51" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Q51" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.3">
@@ -1810,16 +1828,16 @@
         <v>1</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M52">
         <v>0</v>
@@ -1831,10 +1849,10 @@
         <v>1</v>
       </c>
       <c r="P52" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Q52" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
@@ -1851,16 +1869,16 @@
         <v>1</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M53">
         <v>1</v>
@@ -1872,15 +1890,15 @@
         <v>1</v>
       </c>
       <c r="P53" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Q53" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.3">
@@ -1897,16 +1915,16 @@
         <v>1</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M56">
         <v>1</v>
@@ -1918,10 +1936,10 @@
         <v>0</v>
       </c>
       <c r="P56" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Q56" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
@@ -1938,16 +1956,16 @@
         <v>0</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M57">
         <v>1</v>
@@ -1959,10 +1977,10 @@
         <v>0</v>
       </c>
       <c r="P57" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Q57" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.3">
@@ -1979,16 +1997,16 @@
         <v>0</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M58">
         <v>1</v>
@@ -2000,10 +2018,10 @@
         <v>0</v>
       </c>
       <c r="P58" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Q58" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
logic in progress improvemnts. to be updated later
</commit_message>
<xml_diff>
--- a/blue-green/aksrgsample/AKS Upgrade.xlsx
+++ b/blue-green/aksrgsample/AKS Upgrade.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Chaminda\github\terraform_samples\blue-green\aksrgsample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340663CB-EFE2-44B1-8C96-3B84650233DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA6EA93-22E3-4291-8156-2C8CB86BC2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{783D4FFA-E4BF-4C40-98DC-85ACE5E37AF6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="33">
   <si>
     <t>Phase</t>
   </si>
@@ -68,9 +68,6 @@
     <t>green_golive</t>
   </si>
   <si>
-    <t>current_k8s</t>
-  </si>
-  <si>
     <t>tf_k8s</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>010. blue deployment</t>
+  </si>
+  <si>
+    <t>Cluster k8s version</t>
   </si>
 </sst>
 </file>
@@ -150,7 +150,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +175,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -196,7 +202,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -513,49 +519,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D388FFD9-FC26-4C5F-9D9A-2BCDF4241F45}">
-  <dimension ref="A1:Q58"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="15.5546875" customWidth="1"/>
+    <col min="14" max="14" width="14.44140625" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="1"/>
-      <c r="M1" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="J1" s="1"/>
+      <c r="L1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -571,98 +580,83 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
       <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" t="s">
-        <v>13</v>
+      <c r="L2" t="s">
+        <v>7</v>
       </c>
       <c r="M2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -676,34 +670,28 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" t="s">
         <v>6</v>
       </c>
-      <c r="G7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" t="s">
-        <v>6</v>
+      <c r="L7">
+        <v>1</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -719,37 +707,31 @@
       <c r="F8" t="s">
         <v>4</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" t="s">
         <v>6</v>
       </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
       <c r="M8">
         <v>1</v>
       </c>
       <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -765,14 +747,14 @@
       <c r="F11" t="s">
         <v>4</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>4</v>
       </c>
       <c r="I11" t="s">
         <v>4</v>
       </c>
-      <c r="J11" t="s">
-        <v>4</v>
+      <c r="L11">
+        <v>1</v>
       </c>
       <c r="M11">
         <v>1</v>
@@ -780,17 +762,11 @@
       <c r="N11">
         <v>1</v>
       </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
-      <c r="P11" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -806,32 +782,26 @@
       <c r="F12" t="s">
         <v>4</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>4</v>
       </c>
       <c r="I12" t="s">
         <v>4</v>
       </c>
-      <c r="J12" t="s">
-        <v>4</v>
+      <c r="L12">
+        <v>0</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12">
         <v>1</v>
       </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-      <c r="P12" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -847,14 +817,14 @@
       <c r="F13" t="s">
         <v>4</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>4</v>
       </c>
       <c r="I13" t="s">
         <v>4</v>
       </c>
-      <c r="J13" t="s">
-        <v>4</v>
+      <c r="L13">
+        <v>1</v>
       </c>
       <c r="M13">
         <v>1</v>
@@ -862,22 +832,16 @@
       <c r="N13">
         <v>1</v>
       </c>
-      <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="P13" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -893,32 +857,26 @@
       <c r="F16" t="s">
         <v>4</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>4</v>
       </c>
       <c r="I16" t="s">
         <v>4</v>
       </c>
-      <c r="J16" t="s">
-        <v>4</v>
+      <c r="L16">
+        <v>1</v>
       </c>
       <c r="M16">
         <v>1</v>
       </c>
       <c r="N16">
-        <v>1</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -934,32 +892,26 @@
       <c r="F17" t="s">
         <v>4</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>4</v>
       </c>
       <c r="I17" t="s">
         <v>4</v>
       </c>
-      <c r="J17" t="s">
-        <v>4</v>
+      <c r="L17">
+        <v>1</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17">
         <v>0</v>
       </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -975,37 +927,31 @@
       <c r="F18" t="s">
         <v>4</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>4</v>
       </c>
       <c r="I18" t="s">
         <v>4</v>
       </c>
-      <c r="J18" t="s">
-        <v>4</v>
+      <c r="L18">
+        <v>1</v>
       </c>
       <c r="M18">
         <v>1</v>
       </c>
       <c r="N18">
-        <v>1</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -1021,14 +967,14 @@
       <c r="F21" t="s">
         <v>4</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>4</v>
       </c>
       <c r="I21" t="s">
         <v>4</v>
       </c>
-      <c r="J21" t="s">
-        <v>4</v>
+      <c r="L21">
+        <v>1</v>
       </c>
       <c r="M21">
         <v>1</v>
@@ -1036,17 +982,11 @@
       <c r="N21">
         <v>1</v>
       </c>
-      <c r="O21">
-        <v>1</v>
-      </c>
-      <c r="P21" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -1062,32 +1002,26 @@
       <c r="F22" t="s">
         <v>4</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>4</v>
       </c>
       <c r="I22" t="s">
         <v>4</v>
       </c>
-      <c r="J22" t="s">
-        <v>4</v>
+      <c r="L22">
+        <v>0</v>
       </c>
       <c r="M22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22">
         <v>1</v>
       </c>
-      <c r="O22">
-        <v>1</v>
-      </c>
-      <c r="P22" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1103,14 +1037,14 @@
       <c r="F23" t="s">
         <v>4</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>4</v>
       </c>
       <c r="I23" t="s">
         <v>4</v>
       </c>
-      <c r="J23" t="s">
-        <v>4</v>
+      <c r="L23">
+        <v>1</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -1118,22 +1052,16 @@
       <c r="N23">
         <v>1</v>
       </c>
-      <c r="O23">
-        <v>1</v>
-      </c>
-      <c r="P23" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1146,35 +1074,29 @@
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="F26" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" t="s">
-        <v>4</v>
+      <c r="F26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" t="s">
+        <v>4</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
       </c>
       <c r="M26">
         <v>1</v>
       </c>
       <c r="N26">
-        <v>1</v>
-      </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-      <c r="P26" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1187,35 +1109,29 @@
       <c r="D27">
         <v>0</v>
       </c>
-      <c r="F27" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J27" t="s">
-        <v>4</v>
+      <c r="F27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" t="s">
+        <v>4</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
       </c>
       <c r="M27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N27">
         <v>0</v>
       </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1229,39 +1145,33 @@
         <v>0</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" t="s">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
       </c>
       <c r="M28">
         <v>1</v>
       </c>
       <c r="N28">
-        <v>1</v>
-      </c>
-      <c r="O28">
-        <v>0</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -1275,16 +1185,16 @@
         <v>0</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
       </c>
       <c r="M31">
         <v>1</v>
@@ -1292,17 +1202,11 @@
       <c r="N31">
         <v>1</v>
       </c>
-      <c r="O31">
-        <v>1</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -1316,34 +1220,28 @@
         <v>1</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
       </c>
       <c r="M32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N32">
         <v>1</v>
       </c>
-      <c r="O32">
-        <v>1</v>
-      </c>
-      <c r="P32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -1357,16 +1255,16 @@
         <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
       </c>
       <c r="M33">
         <v>1</v>
@@ -1374,22 +1272,16 @@
       <c r="N33">
         <v>1</v>
       </c>
-      <c r="O33">
-        <v>1</v>
-      </c>
-      <c r="P33" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -1403,34 +1295,28 @@
         <v>1</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
       </c>
       <c r="M36">
         <v>1</v>
       </c>
       <c r="N36">
-        <v>1</v>
-      </c>
-      <c r="O36">
-        <v>0</v>
-      </c>
-      <c r="P36" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -1444,34 +1330,28 @@
         <v>0</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
       </c>
       <c r="M37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N37">
         <v>0</v>
       </c>
-      <c r="O37">
-        <v>0</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -1485,62 +1365,56 @@
         <v>0</v>
       </c>
       <c r="F38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="H41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I38" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M38">
-        <v>1</v>
-      </c>
-      <c r="N38">
-        <v>1</v>
-      </c>
-      <c r="O38">
-        <v>0</v>
-      </c>
-      <c r="P38" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>15</v>
+      <c r="L41">
+        <v>1</v>
       </c>
       <c r="M41">
         <v>1</v>
@@ -1548,17 +1422,11 @@
       <c r="N41">
         <v>1</v>
       </c>
-      <c r="O41">
-        <v>1</v>
-      </c>
-      <c r="P41" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -1571,35 +1439,29 @@
       <c r="D42">
         <v>1</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G42" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I42" s="2" t="s">
+      <c r="H42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I42" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J42" s="3" t="s">
-        <v>15</v>
+      <c r="L42">
+        <v>0</v>
       </c>
       <c r="M42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N42">
         <v>1</v>
       </c>
-      <c r="O42">
-        <v>1</v>
-      </c>
-      <c r="P42" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -1613,16 +1475,16 @@
         <v>1</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I43" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J43" s="3" t="s">
-        <v>15</v>
+      <c r="H43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
       </c>
       <c r="M43">
         <v>1</v>
@@ -1630,22 +1492,16 @@
       <c r="N43">
         <v>1</v>
       </c>
-      <c r="O43">
-        <v>1</v>
-      </c>
-      <c r="P43" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -1658,35 +1514,29 @@
       <c r="D46">
         <v>1</v>
       </c>
-      <c r="F46" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J46" s="3" t="s">
-        <v>15</v>
+      <c r="F46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
       </c>
       <c r="M46">
         <v>1</v>
       </c>
       <c r="N46">
-        <v>1</v>
-      </c>
-      <c r="O46">
-        <v>0</v>
-      </c>
-      <c r="P46" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O46" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -1699,35 +1549,29 @@
       <c r="D47">
         <v>0</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>15</v>
+      <c r="F47" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
       </c>
       <c r="M47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N47">
         <v>0</v>
       </c>
-      <c r="O47">
-        <v>0</v>
-      </c>
-      <c r="P47" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -1741,39 +1585,33 @@
         <v>0</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>15</v>
+        <v>15</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
       </c>
       <c r="M48">
         <v>1</v>
       </c>
       <c r="N48">
-        <v>1</v>
-      </c>
-      <c r="O48">
-        <v>0</v>
-      </c>
-      <c r="P48" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O48" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>1</v>
       </c>
@@ -1787,16 +1625,16 @@
         <v>0</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
       </c>
       <c r="M51">
         <v>1</v>
@@ -1804,17 +1642,11 @@
       <c r="N51">
         <v>1</v>
       </c>
-      <c r="O51">
-        <v>1</v>
-      </c>
-      <c r="P51" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q51" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -1828,34 +1660,28 @@
         <v>1</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
       </c>
       <c r="M52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N52">
         <v>1</v>
       </c>
-      <c r="O52">
-        <v>1</v>
-      </c>
-      <c r="P52" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q52" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -1869,16 +1695,16 @@
         <v>1</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
       </c>
       <c r="M53">
         <v>1</v>
@@ -1886,22 +1712,16 @@
       <c r="N53">
         <v>1</v>
       </c>
-      <c r="O53">
-        <v>1</v>
-      </c>
-      <c r="P53" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q53" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>1</v>
       </c>
@@ -1915,34 +1735,28 @@
         <v>1</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J56" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
       </c>
       <c r="M56">
         <v>1</v>
       </c>
       <c r="N56">
-        <v>1</v>
-      </c>
-      <c r="O56">
-        <v>0</v>
-      </c>
-      <c r="P56" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O56" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -1956,34 +1770,28 @@
         <v>0</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J57" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="L57">
+        <v>1</v>
       </c>
       <c r="M57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N57">
         <v>0</v>
       </c>
-      <c r="O57">
-        <v>0</v>
-      </c>
-      <c r="P57" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q57" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O57" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -1997,37 +1805,32 @@
         <v>0</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="L58">
+        <v>1</v>
       </c>
       <c r="M58">
         <v>1</v>
       </c>
       <c r="N58">
-        <v>1</v>
-      </c>
-      <c r="O58">
-        <v>0</v>
-      </c>
-      <c r="P58" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>19</v>
+        <v>0</v>
+      </c>
+      <c r="O58" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="M1:P1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="L1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>